<commit_message>
BLE firmware project added
</commit_message>
<xml_diff>
--- a/Documents/Jegyzetek/Figures/System_design/GATTtable.xlsx
+++ b/Documents/Jegyzetek/Figures/System_design/GATTtable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="417">
   <si>
     <t>0x01</t>
   </si>
@@ -1233,6 +1233,48 @@
   </si>
   <si>
     <t>Disconnect request</t>
+  </si>
+  <si>
+    <t>12:21:00:00:00:00:00:00:00:00:B0:00:40:51:04:01:AA:00:F0</t>
+  </si>
+  <si>
+    <t>IR Temperature Data</t>
+  </si>
+  <si>
+    <t>0A:24:00:00:00:00:00:00:00:00:B0:00:40:51:04:02:AA:00:F0</t>
+  </si>
+  <si>
+    <t>IR Temperature Config</t>
+  </si>
+  <si>
+    <t>0A:26:00:00:00:00:00:00:00:00:B0:00:40:51:04:03:AA:00:F0</t>
+  </si>
+  <si>
+    <t>IR Temperature Period</t>
+  </si>
+  <si>
+    <t>1C:63:00:00:00:00:00:00:00:00:B0:00:40:51:04:C1:FF:00:F0</t>
+  </si>
+  <si>
+    <t>OAT Image Identify</t>
+  </si>
+  <si>
+    <t>OAT Service</t>
+  </si>
+  <si>
+    <t>F000FFC0-0451-4000-B000-000000000000</t>
+  </si>
+  <si>
+    <t>1C:67:00:00:00:00:00:00:00:00:B0:00:40:51:04:C2:FF:00:F0</t>
+  </si>
+  <si>
+    <t>OAT Image Block</t>
+  </si>
+  <si>
+    <t>F000AA00-0451-4000-B000-000000000000</t>
+  </si>
+  <si>
+    <t>IR Temperature Service</t>
   </si>
 </sst>
 </file>
@@ -1556,7 +1598,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1917,8 +1959,12 @@
       <c r="B35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1927,8 +1973,12 @@
       <c r="B36" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1957,8 +2007,12 @@
       <c r="B39" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
+      <c r="C39" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1977,8 +2031,12 @@
       <c r="B41" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -2674,8 +2732,12 @@
       <c r="B100" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
+      <c r="C100" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
@@ -2684,8 +2746,12 @@
       <c r="B101" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
+      <c r="C101" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
@@ -2721,8 +2787,12 @@
       <c r="B105" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
+      <c r="C105" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
@@ -2738,6 +2808,8 @@
       <c r="B107" s="1" t="s">
         <v>332</v>
       </c>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
@@ -2746,6 +2818,8 @@
       <c r="B108" s="1" t="s">
         <v>178</v>
       </c>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
@@ -2754,11 +2828,15 @@
       <c r="B109" s="1" t="s">
         <v>180</v>
       </c>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>181</v>
       </c>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
@@ -2767,6 +2845,8 @@
       <c r="B111" s="1" t="s">
         <v>183</v>
       </c>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
@@ -2775,6 +2855,8 @@
       <c r="B112" s="1" t="s">
         <v>185</v>
       </c>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">

</xml_diff>